<commit_message>
Actualizaciones al plan del proyecto
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/20106065.xlsx
+++ b/tspi/ciclo-1/20106065.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="-315" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Id</t>
   </si>
@@ -185,6 +185,114 @@
   <si>
     <t>Crear la versión final del documento de requerimientos.</t>
   </si>
+  <si>
+    <t>Cada miembro del equipo creo un resumen con los detalles del tutorial.</t>
+  </si>
+  <si>
+    <t>Todos los miembros del equipo han leído los capítulos 1, 2, 3 y el apéndice A del libro Introduction to TSPi.</t>
+  </si>
+  <si>
+    <t>Cada miembro del equipo completó la forma INFO. El equipo llego a un acuerdo con los goles del ciclo 1 y la fecha en que serán entregados los reportes semanales.</t>
+  </si>
+  <si>
+    <t>Todos los miembros del equipo han leído el capítulo 4 del libro Introduction to TSPi. El equipo ha completado el lanzamiento del ciclo #1.</t>
+  </si>
+  <si>
+    <t>El equipo estimó el tamaño y el tiempo de producción de los elementos a producir en el ciclo #1. El equipo definió el diseño conceptual del proyecto y completó la forma STRAT. El equipo documentó los riesgos y problemas encontrados.</t>
+  </si>
+  <si>
+    <t>Todos los miembros del equipo han leído el capítulo 5 del libro Introduction to TSPi. El equipo ha completado la estrategía de desarrollo del ciclo #1.</t>
+  </si>
+  <si>
+    <t>Se completaron las formas TASK y SCHEDULE para el equipo y cada miembro de este. El equipo completo las formas SUMP, SUMQ y SUMS.</t>
+  </si>
+  <si>
+    <t>Se creó la plantilla para la agenda de las reuniones con los clientes.</t>
+  </si>
+  <si>
+    <t>Se creó la plantilla para las minutas de las reuniones con los clientes.</t>
+  </si>
+  <si>
+    <t>Se ha creado la plantilla para las agendas de las reuniones con los cliente.</t>
+  </si>
+  <si>
+    <t>Se creó la agenda para la reunión #1 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se ha creado y enviado la agenda para la reunión #1 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se creó la minuta de la reunión #1 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se creó el esquema del documento de requerimientos.</t>
+  </si>
+  <si>
+    <t>Se ha creado la minuta de la reunión #1 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se identificó y documentó una lista de actores y casos de uso, y de escenarios.</t>
+  </si>
+  <si>
+    <t>Se ha identificado y documentado una lista de actores y casos de uso.</t>
+  </si>
+  <si>
+    <t>Se creó el borrador #1 del diagrama de casos de uso.</t>
+  </si>
+  <si>
+    <t>Se creó el borrador #1 del documento de los escenarios.</t>
+  </si>
+  <si>
+    <t>Se ha creado el borrador #1 del diagrama de casos de uso y del documento de escenarios. Se ha creado el esquema del documento de requerimientos.</t>
+  </si>
+  <si>
+    <t>Se creó el borrador #1 del documento de requerimientos.</t>
+  </si>
+  <si>
+    <t>Se creó la agenda para la reunión #2 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se ha creado y enviado la agenda para la reunión #2 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se creó la minuta de la reunión #2 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se ha creado la minuta de la reunión #2 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se actualizó la lista de actores, casos de uso y de escenarios.</t>
+  </si>
+  <si>
+    <t>Se ha actualizado la lista de actores, casos de uso y escenarios. Se ha creado el borrador #1 del diagrama de casos de uso.</t>
+  </si>
+  <si>
+    <t>Se creó la versión final del diagrama de casos de uso.</t>
+  </si>
+  <si>
+    <t>Se ha creado la versión final del diagrama de casos de uso.</t>
+  </si>
+  <si>
+    <t>Se creó el documento de los casos de uso extendidos.</t>
+  </si>
+  <si>
+    <t>Se ha actualizado la lista de actores, casos de uso y escenarios. Se ha creado el borrador #1 del documento de los escenarios.</t>
+  </si>
+  <si>
+    <t>Se creó la versión final del documento de los escenarios.</t>
+  </si>
+  <si>
+    <t>Se ha creado el borrador #1 del documento de requerimientos. Se ha creado la versión final del diagrama de casos de uso y del documento de escenarios. Se ha creado el documento de los casos de uso extendidos.</t>
+  </si>
+  <si>
+    <t>Se creó la versión final del documento de requerimientos.</t>
+  </si>
+  <si>
+    <t>Cada miembro del equipo ha leído los capítulos 10, 16, 17 y 18 del libro Introduction to TSPi. El equipo ha completado los productos especificados. El equipo ha acumulado toda la información y ha completado todas las formas requeridas.</t>
+  </si>
+  <si>
+    <t>Cada miembro del equipo completó la forma PEER. Se creó el reporte del ciclo correspondiente. Se completaron las formas SUMP y SUMQ para el sistema y todos sus componentes.</t>
+  </si>
 </sst>
 </file>
 
@@ -194,7 +302,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -226,6 +334,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -294,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -358,6 +471,9 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,7 +840,7 @@
   <dimension ref="A1:ALY24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D24"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -774,12 +890,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1013" ht="15">
+    <row r="2" spans="1:1013" ht="25.5">
       <c r="A2" s="16">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22" t="s">
+        <v>56</v>
       </c>
       <c r="E2" s="15">
         <v>7.5</v>
@@ -1817,6 +1937,12 @@
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="C3" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="E3" s="15">
         <v>5</v>
       </c>
@@ -2846,12 +2972,18 @@
       <c r="ALX3" s="11"/>
       <c r="ALY3" s="11"/>
     </row>
-    <row r="4" spans="1:1013" ht="30">
+    <row r="4" spans="1:1013" ht="38.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>37</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="E4" s="15">
         <v>5</v>
@@ -3882,12 +4014,18 @@
       <c r="ALX4" s="11"/>
       <c r="ALY4" s="11"/>
     </row>
-    <row r="5" spans="1:1013" ht="15">
+    <row r="5" spans="1:1013" ht="38.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>38</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="E5" s="15">
         <v>2</v>
@@ -4913,6 +5051,10 @@
       <c r="B6" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22" t="s">
+        <v>63</v>
+      </c>
       <c r="E6" s="15">
         <v>0.5</v>
       </c>
@@ -5937,6 +6079,10 @@
       <c r="B7" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
+        <v>64</v>
+      </c>
       <c r="E7" s="15">
         <v>0.5</v>
       </c>
@@ -6961,6 +7107,12 @@
       <c r="B8" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="C8" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E8" s="15">
         <v>0.5</v>
       </c>
@@ -7978,12 +8130,18 @@
       <c r="ALX8" s="11"/>
       <c r="ALY8" s="11"/>
     </row>
-    <row r="9" spans="1:1013" ht="15">
+    <row r="9" spans="1:1013" ht="25.5">
       <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>42</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="E9" s="15">
         <v>2</v>
@@ -9012,6 +9170,10 @@
       <c r="B10" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="E10" s="15">
         <v>3</v>
       </c>
@@ -10039,6 +10201,8 @@
       <c r="B11" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="15">
         <v>10</v>
       </c>
@@ -11075,6 +11239,8 @@
       <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="15">
         <v>15</v>
       </c>
@@ -12111,6 +12277,12 @@
       <c r="B13" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="C13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>71</v>
+      </c>
       <c r="E13" s="15">
         <v>10</v>
       </c>
@@ -13146,6 +13318,12 @@
       </c>
       <c r="B14" s="5" t="s">
         <v>47</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="E14" s="15">
         <v>2</v>
@@ -14174,6 +14352,12 @@
       <c r="B15" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="C15" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="E15" s="15">
         <v>2</v>
       </c>
@@ -15191,12 +15375,18 @@
       <c r="ALX15" s="11"/>
       <c r="ALY15" s="11"/>
     </row>
-    <row r="16" spans="1:1013" ht="30">
+    <row r="16" spans="1:1013" ht="38.25">
       <c r="A16" s="16">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>49</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -16225,6 +16415,12 @@
       <c r="B17" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="C17" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>77</v>
+      </c>
       <c r="E17" s="15">
         <v>0.5</v>
       </c>
@@ -17242,12 +17438,18 @@
       <c r="ALX17" s="11"/>
       <c r="ALY17" s="11"/>
     </row>
-    <row r="18" spans="1:1013" ht="15">
+    <row r="18" spans="1:1013" ht="25.5">
       <c r="A18" s="16">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>51</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="E18" s="15">
         <v>2</v>
@@ -18276,6 +18478,12 @@
       <c r="B19" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="C19" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="E19" s="15">
         <v>10</v>
       </c>
@@ -19305,12 +19513,18 @@
       <c r="ALX19" s="11"/>
       <c r="ALY19" s="11"/>
     </row>
-    <row r="20" spans="1:1013" ht="30">
+    <row r="20" spans="1:1013" ht="38.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="E20" s="15">
         <v>2</v>
@@ -20329,12 +20543,18 @@
       <c r="ALX20" s="11"/>
       <c r="ALY20" s="11"/>
     </row>
-    <row r="21" spans="1:1013" ht="15">
+    <row r="21" spans="1:1013" ht="25.5">
       <c r="A21" s="16">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>53</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="E21" s="15">
         <v>3</v>
@@ -21356,12 +21576,18 @@
       <c r="ALX21" s="11"/>
       <c r="ALY21" s="11"/>
     </row>
-    <row r="22" spans="1:1013" ht="30">
+    <row r="22" spans="1:1013" ht="38.25">
       <c r="A22" s="16">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>54</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="E22" s="15">
         <v>2</v>
@@ -22383,12 +22609,18 @@
       <c r="ALX22" s="11"/>
       <c r="ALY22" s="11"/>
     </row>
-    <row r="23" spans="1:1013" ht="30">
+    <row r="23" spans="1:1013" ht="51">
       <c r="A23" s="16">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>55</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="E23" s="15">
         <v>4</v>
@@ -23410,12 +23642,18 @@
       <c r="ALX23" s="11"/>
       <c r="ALY23" s="11"/>
     </row>
-    <row r="24" spans="1:1013" ht="30">
+    <row r="24" spans="1:1013" ht="63.75">
       <c r="A24" s="16">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>33</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="E24" s="15">
         <v>5</v>

</xml_diff>